<commit_message>
Added business rules with scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Payment Data Integrity\UPO\UPO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POC\workspace\workspace\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F434CCB-9229-43E7-ABE0-4E22EC4BAACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566369F6-D97B-4DF4-8452-5EC29019E37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>RuleSet</t>
   </si>
@@ -63,56 +63,116 @@
     <t>PRIORITY</t>
   </si>
   <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>upo:Upo()</t>
+  </si>
+  <si>
+    <t>FED</t>
+  </si>
+  <si>
+    <t>CHIPS</t>
+  </si>
+  <si>
+    <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getCdtrAgt().getComWellsfargoEpdUpoAvroCdtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("$param");</t>
+  </si>
+  <si>
+    <t>Greater than USD100 CR</t>
+  </si>
+  <si>
+    <t>Greater thann USD200 CR</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Uschu</t>
+  </si>
+  <si>
+    <t>upo.pmtInf.comWellsfargoEpdUpoAvroPmtInf.amt.comWellsfargoEpdUpoAvroAmt.cdtAmt.comWellsfargoEpdUpoAvroCdtAmt.amt.amount&gt; $param</t>
+  </si>
+  <si>
+    <t>FED_1</t>
+  </si>
+  <si>
+    <t>CHIPS_1</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>System.out.println($param);</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>"The amount is more than 100"</t>
+  </si>
+  <si>
+    <t>"The amount is more than 200"</t>
+  </si>
+  <si>
+    <t>"The amount is more than 300"</t>
+  </si>
+  <si>
+    <t>"The amount is more than 400"</t>
+  </si>
+  <si>
     <t>AGENDA-GROUP</t>
   </si>
   <si>
-    <t>CONDITION</t>
-  </si>
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>CREDIT</t>
-  </si>
-  <si>
-    <t>upo: Upo()</t>
-  </si>
-  <si>
-    <t>DEBIT</t>
-  </si>
-  <si>
-    <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getDbtrAgt().getComWellsfargoEpdUpoAvroDbtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("DT_FED");</t>
-  </si>
-  <si>
-    <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getDbtrAgt().getComWellsfargoEpdUpoAvroDbtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("DT_CHIPS");</t>
-  </si>
-  <si>
-    <t>pmtInf.com_wellsfargo_epd_upo_avro_PmtInf.amt.com_wellsfargo_epd_upo_avro_Amt.dbtAmt.com_wellsfargo_epd_upo_avro_DbtAmt.amt.amount&gt; 100</t>
-  </si>
-  <si>
-    <t>pmtInf.com_wellsfargo_epd_upo_avro_PmtInf.amt.com_wellsfargo_epd_upo_avro_Amt.cdtAmt.com_wellsfargo_epd_upo_avro_CdtAmt.amt.amount&gt; 200</t>
-  </si>
-  <si>
-    <t>pmtInf.com_wellsfargo_epd_upo_avro_PmtInf.amt.com_wellsfargo_epd_upo_avro_Amt.cdtAmt.com_wellsfargo_epd_upo_avro_CdtAmt.amt.amount&gt; 100</t>
-  </si>
-  <si>
-    <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getCdtrAgt().getComWellsfargoEpdUpoAvroCdtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("FED");</t>
-  </si>
-  <si>
-    <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getCdtrAgt().getComWellsfargoEpdUpoAvroCdtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("CHIPS");</t>
-  </si>
-  <si>
-    <t>Greater thann USD100</t>
-  </si>
-  <si>
-    <t>Greater thann USD200</t>
+    <t>ACTIVATION-GROUP</t>
+  </si>
+  <si>
+    <t>Greater thann USD300 DT</t>
+  </si>
+  <si>
+    <t>Greater thann USD400 DT</t>
+  </si>
+  <si>
+    <t>"The amount is more than 500"</t>
+  </si>
+  <si>
+    <t>"The amount is more than 600"</t>
+  </si>
+  <si>
+    <t>FED_2</t>
+  </si>
+  <si>
+    <t>CHIPS_2</t>
+  </si>
+  <si>
+    <t>ABCMGUG1</t>
+  </si>
+  <si>
+    <t>Greater thann USD500 for ABCMGUG1</t>
+  </si>
+  <si>
+    <t>Greater thann USD600 for ABCMGUG1</t>
+  </si>
+  <si>
+    <t>ABCMGUG2</t>
+  </si>
+  <si>
+    <t>Greater than USD50 CR</t>
+  </si>
+  <si>
+    <t>FED_0</t>
+  </si>
+  <si>
+    <t>"The amount is more than 50"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,21 +190,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,8 +223,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,11 +241,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
@@ -269,43 +316,48 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
+    <cellStyle name="Excel Built-in Normal" xfId="4" xr:uid="{B2538F6E-6FE9-4D4C-B884-0D82A02213FE}"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -617,169 +669,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72884151-AA33-4114-8285-349E17DA6D86}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="34.90625" customWidth="1"/>
+    <col min="6" max="6" width="31.453125" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="F8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="G8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10" s="9">
+        <v>50</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>23</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="9">
+        <v>100</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D13" s="8"/>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9">
+        <v>200</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="9">
+        <v>300</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="9">
+        <v>400</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="10">
+        <v>500</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="10">
+        <v>600</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the runtime errors after merge
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POC\workspace\workspace\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A9841E-BCF9-429D-BF1E-59B6DABBC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA91F180-3C7A-4CC2-B11D-A00EB2876DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>RuleSet</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>"The amount is more than 50"</t>
+  </si>
+  <si>
+    <t>Greater thann USD500 for ABCMGUG2</t>
+  </si>
+  <si>
+    <t>Greater thann USD600 for ABCMGUG2</t>
   </si>
 </sst>
 </file>
@@ -672,7 +678,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,7 +948,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -962,13 +968,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E18" s="10">
         <v>600</v>

</xml_diff>

<commit_message>
Deleted First rule from upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POC\workspace\workspace\rbms\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA91F180-3C7A-4CC2-B11D-A00EB2876DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49702CA5-54FF-469C-9F47-6BA2DCF10269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>RuleSet</t>
   </si>
@@ -157,15 +157,6 @@
   </si>
   <si>
     <t>ABCMGUG2</t>
-  </si>
-  <si>
-    <t>Greater than USD50 CR</t>
-  </si>
-  <si>
-    <t>FED_0</t>
-  </si>
-  <si>
-    <t>"The amount is more than 50"</t>
   </si>
   <si>
     <t>Greater thann USD500 for ABCMGUG2</t>
@@ -326,7 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,7 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -675,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72884151-AA33-4114-8285-349E17DA6D86}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,182 +797,163 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10"/>
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
       <c r="E10" s="9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E12" s="9">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
       <c r="E13" s="9">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="9">
-        <v>400</v>
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="10">
+        <v>500</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E16" s="10">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="10">
-        <v>600</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted 1 more rule from upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49702CA5-54FF-469C-9F47-6BA2DCF10269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B203B8A7-EA95-40F9-BFF2-E218BBCF8841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>RuleSet</t>
   </si>
@@ -75,18 +75,12 @@
     <t>FED</t>
   </si>
   <si>
-    <t>CHIPS</t>
-  </si>
-  <si>
     <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getCdtrAgt().getComWellsfargoEpdUpoAvroCdtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("$param");</t>
   </si>
   <si>
     <t>Greater than USD100 CR</t>
   </si>
   <si>
-    <t>Greater thann USD200 CR</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
   </si>
   <si>
     <t>"The amount is more than 100"</t>
-  </si>
-  <si>
-    <t>"The amount is more than 200"</t>
   </si>
   <si>
     <t>"The amount is more than 300"</t>
@@ -665,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72884151-AA33-4114-8285-349E17DA6D86}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,16 +727,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>10</v>
@@ -763,13 +754,13 @@
     </row>
     <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="E8" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -782,36 +773,36 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" s="9">
         <v>100</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
@@ -819,7 +810,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -828,133 +819,113 @@
         <v>37</v>
       </c>
       <c r="E11" s="9">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E12" s="9">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="10">
+        <v>500</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="9">
-        <v>400</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
         <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="10">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E16" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
         <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="10">
-        <v>600</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted another rule from upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B203B8A7-EA95-40F9-BFF2-E218BBCF8841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292FC81D-4C28-48FE-AFA9-EC2DC8345F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>RuleSet</t>
   </si>
@@ -72,15 +72,9 @@
     <t>upo:Upo()</t>
   </si>
   <si>
-    <t>FED</t>
-  </si>
-  <si>
     <t>upo.getPmtInf().getComWellsfargoEpdUpoAvroPmtInf().getCdtrAgt().getComWellsfargoEpdUpoAvroCdtrAgt().getFinInstnId2().getComWellsfargoEpdUpoAvroFinInstnId2().setUschu("$param");</t>
   </si>
   <si>
-    <t>Greater than USD100 CR</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
   </si>
   <si>
     <t>Log</t>
-  </si>
-  <si>
-    <t>"The amount is more than 100"</t>
   </si>
   <si>
     <t>"The amount is more than 300"</t>
@@ -656,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72884151-AA33-4114-8285-349E17DA6D86}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -727,16 +718,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>10</v>
@@ -754,13 +745,13 @@
     </row>
     <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="E8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -773,159 +764,139 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="9">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="9">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10">
+        <v>500</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
         <v>29</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="9">
-        <v>400</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="10">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="10">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
         <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="10">
-        <v>600</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Action values in upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40E573-8014-4AEE-889E-C33BE1264696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F414D8C-C306-48EC-B359-03DF251E355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -135,22 +135,22 @@
     <t>Greater thann USD600 for ABCMGUG2</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72884151-AA33-4114-8285-349E17DA6D86}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated values in upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F414D8C-C306-48EC-B359-03DF251E355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB8BC48-D608-47CB-A306-669A0727EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -135,22 +135,22 @@
     <t>Greater thann USD600 for ABCMGUG2</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated new values in upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB8BC48-D608-47CB-A306-669A0727EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61698DED-3853-47FC-BD5B-42007A9FB3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -135,22 +135,22 @@
     <t>Greater thann USD600 for ABCMGUG2</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated new value 'A' in upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61698DED-3853-47FC-BD5B-42007A9FB3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A34B45-5578-451A-97DB-0B9E2D87CAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>k</t>
   </si>
   <si>
-    <t>l</t>
+    <t>A</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated new value 'B' in upo-agenda-rules.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/upo-agenda-rules.xlsx
+++ b/src/main/resources/rules/upo-agenda-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rbms\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A34B45-5578-451A-97DB-0B9E2D87CAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B605B14-5A6F-4822-A616-3617082680D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26DAF916-A995-4D32-B12C-1AF365350058}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>k</t>
   </si>
   <si>
-    <t>A</t>
+    <t>B</t>
   </si>
 </sst>
 </file>

</xml_diff>